<commit_message>
Implementado a identifcação do numero desenhado pela Rede Neural
</commit_message>
<xml_diff>
--- a/PlanilhaResultados.xlsx
+++ b/PlanilhaResultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougl\Documents\Github\redes-neurais-digitos-manuscritos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BF3C49-FF03-4634-ADC6-8603DB437A21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9EDE8E-9436-4F31-957B-BCE5FEB7F1E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{3F5FA227-1D17-416F-B661-F542DD628BAF}"/>
   </bookViews>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
-  <si>
-    <t>Modelo de Vaidação Cruzada</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>acurácia</t>
   </si>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>Camada 3</t>
+  </si>
+  <si>
+    <t>Camada 4</t>
+  </si>
+  <si>
+    <t>Modelo de Validação Cruzada</t>
   </si>
 </sst>
 </file>
@@ -153,15 +156,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,26 +169,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,261 +516,269 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="13" style="10" customWidth="1"/>
-    <col min="9" max="9" width="12" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="H1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" s="8" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="H1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="H3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="16">
-        <v>50</v>
-      </c>
-      <c r="J3" s="16"/>
+      <c r="H3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11">
+        <v>60</v>
+      </c>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="H4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="16">
+      <c r="H4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="11">
         <v>50</v>
       </c>
-      <c r="J4" s="16"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="H5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="16">
-        <v>25</v>
-      </c>
-      <c r="J5" s="16"/>
+      <c r="H5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="11">
+        <v>50</v>
+      </c>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
+      <c r="H6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="11">
+        <v>80</v>
+      </c>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="H10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="H10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J11" s="14"/>
-      <c r="M11" s="17"/>
+      <c r="M11" s="10"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="12">
         <v>1</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="H12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="16">
+      <c r="H12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="11">
         <v>50</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="12">
         <v>2</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="H13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="16">
+      <c r="H13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="11">
         <v>50</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="12">
         <v>3</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="H14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="16">
+      <c r="H14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="11">
         <v>25</v>
       </c>
-      <c r="J14" s="16"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="12">
         <v>4</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="12">
         <v>5</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>